<commit_message>
Atualizações e algumas conexões
</commit_message>
<xml_diff>
--- a/wiki/CronogramaKlass.xlsx
+++ b/wiki/CronogramaKlass.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072907B4-678C-4476-9851-3E5C5C19EA3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83CB738-7D5C-4DED-B98D-AA5BB585FBCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8301,7 +8301,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="6"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="26"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10548,7 +10548,7 @@
       <c r="M3" s="6"/>
       <c r="N3" s="35">
         <f ca="1">TODAY()-DATE(2020, 7, 5)-7</f>
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="O3" s="35"/>
       <c r="P3" s="6"/>
@@ -14002,7 +14002,7 @@
   <dimension ref="B2:BR36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>
@@ -14047,7 +14047,7 @@
       <c r="M3" s="6"/>
       <c r="N3" s="35">
         <f ca="1">TODAY()-DATE(2020, 9, 13)</f>
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="O3" s="35"/>
       <c r="P3" s="6"/>
@@ -14357,7 +14357,7 @@
         <v>7</v>
       </c>
       <c r="H9" s="14">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="BR9" s="1"/>
     </row>
@@ -14381,7 +14381,7 @@
         <v>14</v>
       </c>
       <c r="H10" s="14">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="AD10"/>
       <c r="AE10"/>
@@ -14445,7 +14445,7 @@
         <v>7</v>
       </c>
       <c r="H11" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD11"/>
       <c r="AE11"/>
@@ -14509,7 +14509,7 @@
         <v>7</v>
       </c>
       <c r="H12" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD12"/>
       <c r="AE12"/>
@@ -14558,7 +14558,7 @@
         <v>92</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" s="13">
         <v>22</v>
@@ -14637,7 +14637,7 @@
         <v>14</v>
       </c>
       <c r="H14" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD14"/>
       <c r="AE14"/>
@@ -14701,7 +14701,7 @@
         <v>7</v>
       </c>
       <c r="H15" s="14">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:70" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -14724,7 +14724,7 @@
         <v>7</v>
       </c>
       <c r="H16" s="23">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="I16" s="24"/>
       <c r="J16" s="24"/>
@@ -14793,7 +14793,7 @@
         <v>96</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D17" s="22">
         <v>15</v>
@@ -14808,7 +14808,7 @@
         <v>7</v>
       </c>
       <c r="H17" s="23">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="I17" s="24"/>
       <c r="J17" s="24"/>
@@ -14961,7 +14961,7 @@
         <v>97</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" s="22">
         <v>22</v>
@@ -15060,7 +15060,7 @@
         <v>14</v>
       </c>
       <c r="H20" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="24"/>
       <c r="J20" s="24"/>
@@ -15144,7 +15144,7 @@
         <v>7</v>
       </c>
       <c r="H21" s="23">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="I21" s="24"/>
       <c r="J21" s="24"/>
@@ -15228,7 +15228,7 @@
         <v>7</v>
       </c>
       <c r="H22" s="14">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="23" spans="2:69" x14ac:dyDescent="0.35">
@@ -15236,7 +15236,7 @@
         <v>100</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D23" s="13">
         <v>29</v>
@@ -15251,7 +15251,7 @@
         <v>14</v>
       </c>
       <c r="H23" s="14">
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="24" spans="2:69" x14ac:dyDescent="0.35">

</xml_diff>